<commit_message>
[UPDATE] modify calculating conductivity
</commit_message>
<xml_diff>
--- a/Building_Energy_Prediction_Project/data/lhs_sample/interval.xlsx
+++ b/Building_Energy_Prediction_Project/data/lhs_sample/interval.xlsx
@@ -5,49 +5,38 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwchoi0610\dongwook\서울기술연구원\관련파일\Building_Energy_Prediction_Project\Building_Energy_Prediction_Project\data\lhs_sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dwcho\dongwook\Building_Energy_Prediction_Project\Building_Energy_Prediction_Project\data\lhs_sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329BE6D3-A644-4D9D-8E87-DBDD11F8C5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF99496-E42C-4104-BD4D-A6FBC05BE259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="20650" windowHeight="18420" activeTab="4" xr2:uid="{A0916A1B-620D-4006-A6C2-ACBE89CA4642}"/>
+    <workbookView xWindow="9315" yWindow="2910" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{A0916A1B-620D-4006-A6C2-ACBE89CA4642}"/>
   </bookViews>
   <sheets>
     <sheet name="Facade" sheetId="1" r:id="rId1"/>
-    <sheet name="Ground(Off,Ret)" sheetId="2" r:id="rId2"/>
-    <sheet name="Ground(Res)" sheetId="3" r:id="rId3"/>
-    <sheet name="Roof" sheetId="4" r:id="rId4"/>
+    <sheet name="Ground" sheetId="4" r:id="rId2"/>
+    <sheet name="Roof(Off,Ret)" sheetId="2" r:id="rId3"/>
+    <sheet name="Roof(Res)" sheetId="3" r:id="rId4"/>
     <sheet name="Window" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -432,14 +421,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238C74BC-7CEC-4416-BAF8-47EB7117ED01}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -727,7 +716,7 @@
         <v>0.66939999999999933</v>
       </c>
       <c r="B32">
-        <f t="shared" si="0"/>
+        <f>1/(0.360091+A32/0.037)</f>
         <v>5.4194717492363244E-2</v>
       </c>
     </row>
@@ -909,477 +898,477 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E60C871-246C-48E4-BAE9-694B95CA5DC7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878CD215-E8A8-4291-91D1-D9B971EA1525}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" cm="1">
-        <f t="array" ref="A1:A51">_xlfn.SEQUENCE(51, 1, 0.13, (1 - 0.13) / (51 - 1))</f>
-        <v>0.13</v>
+        <f t="array" ref="A1:A51">_xlfn.SEQUENCE(51, 1, 0.17, (1 - 0.17) / (51 - 1))</f>
+        <v>0.17</v>
       </c>
       <c r="B1">
-        <f>1/(0.544481+A1/0.037)</f>
-        <v>0.24642714441084224</v>
+        <f>1/(0.172457+A1/0.037)</f>
+        <v>0.20977326973635227</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>0.1474</v>
+        <v>0.18660000000000002</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B51" si="0">1/(0.544481+A2/0.037)</f>
-        <v>0.22083514276398111</v>
+        <f t="shared" ref="B2:B51" si="0">1/(0.172457+A2/0.037)</f>
+        <v>0.19172880981714102</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>0.1648</v>
+        <v>0.20320000000000002</v>
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>0.20005861501140246</v>
+        <v>0.17654279760758171</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>0.1822</v>
+        <v>0.21980000000000002</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>0.18285529301110218</v>
+        <v>0.16358586656842905</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>0.1996</v>
+        <v>0.23640000000000003</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>0.16837637172191283</v>
+        <v>0.15240078040897356</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>0.217</v>
+        <v>0.253</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>0.15602216218067738</v>
+        <v>0.14264735266233491</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>0.2344</v>
+        <v>0.26960000000000001</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>0.14535694730013554</v>
+        <v>0.13406724448465382</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>0.25180000000000002</v>
+        <v>0.28620000000000001</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>0.13605652452867287</v>
+        <v>0.12646074594019394</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>0.26919999999999999</v>
+        <v>0.30280000000000001</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>0.12787467585022497</v>
+        <v>0.11967103699795384</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>0.28659999999999997</v>
+        <v>0.31940000000000002</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>0.12062104961783715</v>
+        <v>0.11357326036560356</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>0.30399999999999994</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>0.11414616614634064</v>
+        <v>0.1080667730805049</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>0.32139999999999991</v>
+        <v>0.35260000000000002</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>0.10833100663217943</v>
+        <v>0.10306954791292257</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>0.33879999999999988</v>
+        <v>0.36920000000000003</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>0.10307963015374159</v>
+        <v>9.8514059456626946E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>0.35619999999999985</v>
+        <v>0.38580000000000003</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>9.8313838748676163E-2</v>
+        <v>9.4344215006141458E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>0.37359999999999982</v>
+        <v>0.40240000000000004</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>9.3969257022951835E-2</v>
+        <v>9.0513033229739207E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>0.39099999999999979</v>
+        <v>0.41900000000000004</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>8.9992407243311839E-2</v>
+        <v>8.6980866365114651E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>0.40839999999999976</v>
+        <v>0.43560000000000004</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>8.6338496979822252E-2</v>
+        <v>8.3714023041660368E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>0.42579999999999973</v>
+        <v>0.45220000000000005</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>8.2969724681585061E-2</v>
+        <v>8.0683690214413156E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>0.44319999999999971</v>
+        <v>0.46880000000000005</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>7.9853967036200443E-2</v>
+        <v>7.786508106536745E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>0.46059999999999968</v>
+        <v>0.48540000000000005</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>7.6963751385641391E-2</v>
+        <v>7.5236755479664214E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>0.47799999999999965</v>
+        <v>0.502</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>7.427544350032933E-2</v>
+        <v>7.2780073651428162E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>0.49539999999999962</v>
+        <v>0.51859999999999995</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>7.1768599832072774E-2</v>
+        <v>7.0478753352152854E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>0.51279999999999959</v>
+        <v>0.5351999999999999</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>6.9425446655694389E-2</v>
+        <v>6.8318508620103538E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>0.53019999999999956</v>
+        <v>0.55179999999999985</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>6.7230458016925732E-2</v>
+        <v>6.6286752920816941E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>0.54759999999999953</v>
+        <v>0.56839999999999979</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>6.5170011289401114E-2</v>
+        <v>6.4372353744964084E-2</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>0.5649999999999995</v>
+        <v>0.58499999999999974</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>6.3232104186164109E-2</v>
+        <v>6.2565428536686188E-2</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>0.58239999999999947</v>
+        <v>0.60159999999999969</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>6.1406120803129648E-2</v>
+        <v>6.0857174053141214E-2</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>0.59979999999999944</v>
+        <v>0.61819999999999964</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>5.968263706125268E-2</v>
+        <v>5.9239722935559687E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>0.61719999999999942</v>
+        <v>0.63479999999999959</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>5.8053258018111689E-2</v>
+        <v>5.7706022560319273E-2</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>0.63459999999999939</v>
+        <v>0.65139999999999953</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>5.6510481120354603E-2</v>
+        <v>5.6249732234171644E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>0.65199999999999936</v>
+        <v>0.66799999999999948</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>5.5047580696245921E-2</v>
+        <v>5.4865135572810267E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>0.66939999999999933</v>
+        <v>0.68459999999999943</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>5.3658509936505387E-2</v>
+        <v>5.3547065509446698E-2</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>0.6867999999999993</v>
+        <v>0.70119999999999938</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>5.2337817350373225E-2</v>
+        <v>5.2290839859276121E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>0.70419999999999927</v>
+        <v>0.71779999999999933</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>5.1080575262867203E-2</v>
+        <v>5.1092205746064517E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>0.72159999999999924</v>
+        <v>0.73439999999999928</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>4.9882318375981352E-2</v>
+        <v>4.9947291500731739E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>0.73899999999999921</v>
+        <v>0.75099999999999922</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>4.8738990779132289E-2</v>
+        <v>4.8852564885550918E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>0.75639999999999918</v>
+        <v>0.76759999999999917</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>4.7646900083601937E-2</v>
+        <v>4.7804796694281303E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>0.77379999999999916</v>
+        <v>0.78419999999999912</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>4.6602677588077256E-2</v>
+        <v>4.6801028938076764E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>0.79119999999999913</v>
+        <v>0.80079999999999907</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>4.5603243569893093E-2</v>
+        <v>4.5838546957011887E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>0.8085999999999991</v>
+        <v>0.81739999999999902</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>4.4645776948658282E-2</v>
+        <v>4.4914854903489933E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>0.82599999999999907</v>
+        <v>0.83399999999999896</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>4.3727688692874328E-2</v>
+        <v>4.402765413130065E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>0.84339999999999904</v>
+        <v>0.85059999999999891</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>4.2846598441611122E-2</v>
+        <v>4.3174824096344065E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>0.86079999999999901</v>
+        <v>0.86719999999999886</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>4.200031389672438E-2</v>
+        <v>4.2354405434929264E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>0.87819999999999898</v>
+        <v>0.88379999999999881</v>
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>4.1186812609977669E-2</v>
+        <v>4.1564584935397719E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>0.89559999999999895</v>
+        <v>0.90039999999999876</v>
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>4.0404225846531555E-2</v>
+        <v>4.0803682160450119E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>0.91299999999999892</v>
+        <v>0.91699999999999871</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>3.965082425377954E-2</v>
+        <v>4.0070137512448881E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>0.93039999999999889</v>
+        <v>0.93359999999999865</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>3.8925005104199141E-2</v>
+        <v>3.9362501563316381E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>0.94779999999999887</v>
+        <v>0.9501999999999986</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>3.8225280914154371E-2</v>
+        <v>3.8679425495413117E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>0.96519999999999884</v>
+        <v>0.96679999999999855</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>3.7550269268566271E-2</v>
+        <v>3.8019652520742214E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>0.98259999999999881</v>
+        <v>0.9833999999999985</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>3.6898683704978959E-2</v>
+        <v>3.7382010163625065E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>0.99999999999999878</v>
+        <v>0.99999999999999845</v>
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>3.6269325530534968E-2</v>
+        <v>3.6765403307148836E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1389,17 +1378,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DDF6F6-46C1-4FA8-923D-47BEB7A5CA44}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E60C871-246C-48E4-BAE9-694B95CA5DC7}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1408,8 +1397,8 @@
         <v>0.13</v>
       </c>
       <c r="B1">
-        <f>1/(0.510281+A1/0.037)</f>
-        <v>0.24852163713668768</v>
+        <f>1/(0.544481+A1/0.037)</f>
+        <v>0.24642714441084224</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1417,8 +1406,8 @@
         <v>0.1474</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B51" si="0">1/(0.510281+A2/0.037)</f>
-        <v>0.22251570640645027</v>
+        <f t="shared" ref="B2:B51" si="0">1/(0.544481+A2/0.037)</f>
+        <v>0.22083514276398111</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1427,7 +1416,7 @@
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>0.20143684685089175</v>
+        <v>0.20005861501140246</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1436,7 +1425,7 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>0.18400600233547382</v>
+        <v>0.18285529301110218</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1445,7 +1434,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>0.16935157802738704</v>
+        <v>0.16837637172191283</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1454,7 +1443,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>0.15685915604084727</v>
+        <v>0.15602216218067738</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1463,7 +1452,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>0.1460831570001053</v>
+        <v>0.14535694730013554</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1472,7 +1461,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>0.13669257327119996</v>
+        <v>0.13605652452867287</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1481,7 +1470,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>0.12843636840725403</v>
+        <v>0.12787467585022497</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1490,7 +1479,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>0.12112070156829081</v>
+        <v>0.12062104961783715</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1499,7 +1488,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>0.11459351618673833</v>
+        <v>0.11414616614634064</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1508,7 +1497,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>0.10873385691976843</v>
+        <v>0.10833100663217943</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1517,7 +1506,7 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>0.10344430477692633</v>
+        <v>0.10307963015374159</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1526,7 +1515,7 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>9.8645517856802326E-2</v>
+        <v>9.8313838748676163E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1535,7 +1524,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>9.4272224250731201E-2</v>
+        <v>9.3969257022951835E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1544,7 +1533,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>9.0270235587773209E-2</v>
+        <v>8.9992407243311839E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1553,7 +1542,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>8.6594190278287006E-2</v>
+        <v>8.6338496979822252E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1562,7 +1551,7 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>8.3205826588303639E-2</v>
+        <v>8.2969724681585061E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1571,7 +1560,7 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>8.0072645886339167E-2</v>
+        <v>7.9853967036200443E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1580,7 +1569,7 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>7.7166866949098689E-2</v>
+        <v>7.6963751385641391E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1589,7 +1578,7 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>7.4464599978976476E-2</v>
+        <v>7.427544350032933E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1598,7 +1587,7 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>7.1945188297737162E-2</v>
+        <v>7.1768599832072774E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1607,7 +1596,7 @@
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>6.9590679304281408E-2</v>
+        <v>6.9425446655694389E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1616,7 +1605,7 @@
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>6.7385396022433527E-2</v>
+        <v>6.7230458016925732E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1625,7 +1614,7 @@
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>6.5315587610704245E-2</v>
+        <v>6.5170011289401114E-2</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1634,7 +1623,7 @@
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>6.3369142362215705E-2</v>
+        <v>6.3232104186164109E-2</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1643,7 +1632,7 @@
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>6.1535350536299008E-2</v>
+        <v>6.1406120803129648E-2</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1652,7 +1641,7 @@
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>5.9804707211371426E-2</v>
+        <v>5.968263706125268E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1661,7 +1650,7 @@
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>5.8168747495609484E-2</v>
+        <v>5.8053258018111689E-2</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1670,7 +1659,7 @@
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>5.6619908064357793E-2</v>
+        <v>5.6510481120354603E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1679,7 +1668,7 @@
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>5.5151410244589444E-2</v>
+        <v>5.5047580696245921E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1688,7 +1677,7 @@
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>5.3757160833392201E-2</v>
+        <v>5.3658509936505387E-2</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1697,7 +1686,7 @@
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>5.2431667589598684E-2</v>
+        <v>5.2337817350373225E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1706,7 +1695,7 @@
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>5.1169966926928094E-2</v>
+        <v>5.1080575262867203E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1715,7 +1704,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>4.9967561801639478E-2</v>
+        <v>4.9882318375981352E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1724,7 +1713,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>4.8820368156322742E-2</v>
+        <v>4.8738990779132289E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1733,7 +1722,7 @@
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>4.7724668575619918E-2</v>
+        <v>4.7646900083601937E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1742,7 +1731,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>4.6677072045721392E-2</v>
+        <v>4.6602677588077256E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1751,7 +1740,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>4.5674478899901137E-2</v>
+        <v>4.5603243569893093E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1760,7 +1749,7 @@
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>4.4714050186738186E-2</v>
+        <v>4.4645776948658282E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1769,7 +1758,7 @@
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>4.379318082343913E-2</v>
+        <v>4.3727688692874328E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1778,7 +1767,7 @@
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>4.2909475999603458E-2</v>
+        <v>4.2846598441611122E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1787,7 +1776,7 @@
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>4.2060730381377406E-2</v>
+        <v>4.200031389672438E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1796,7 +1785,7 @@
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>4.1244909735777047E-2</v>
+        <v>4.1186812609977669E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1805,7 +1794,7 @@
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>4.0460134652837224E-2</v>
+        <v>4.0404225846531555E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1814,7 +1803,7 @@
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>3.9704666091393316E-2</v>
+        <v>3.965082425377954E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1823,7 +1812,7 @@
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>3.8976892514509642E-2</v>
+        <v>3.8925005104199141E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1832,7 +1821,7 @@
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>3.8275318414261836E-2</v>
+        <v>3.8225280914154371E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1841,7 +1830,7 @@
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>3.7598554053912367E-2</v>
+        <v>3.7550269268566271E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1850,7 +1839,7 @@
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>3.6945306279419908E-2</v>
+        <v>3.6898683704978959E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1859,7 +1848,7 @@
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>3.6314370272451164E-2</v>
+        <v>3.6269325530534968E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1869,477 +1858,477 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{878CD215-E8A8-4291-91D1-D9B971EA1525}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DDF6F6-46C1-4FA8-923D-47BEB7A5CA44}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" cm="1">
-        <f t="array" ref="A1:A51">_xlfn.SEQUENCE(51, 1, 0.17, (1 - 0.17) / (51 - 1))</f>
-        <v>0.17</v>
+        <f t="array" ref="A1:A51">_xlfn.SEQUENCE(51, 1, 0.13, (1 - 0.13) / (51 - 1))</f>
+        <v>0.13</v>
       </c>
       <c r="B1">
-        <f>1/(0.172457+A1/0.037)</f>
-        <v>0.20977326973635227</v>
+        <f>1/(0.510281+A1/0.037)</f>
+        <v>0.24852163713668768</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>0.18660000000000002</v>
+        <v>0.1474</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B51" si="0">1/(0.172457+A2/0.037)</f>
-        <v>0.19172880981714102</v>
+        <f t="shared" ref="B2:B51" si="0">1/(0.510281+A2/0.037)</f>
+        <v>0.22251570640645027</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>0.20320000000000002</v>
+        <v>0.1648</v>
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>0.17654279760758171</v>
+        <v>0.20143684685089175</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>0.21980000000000002</v>
+        <v>0.1822</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>0.16358586656842905</v>
+        <v>0.18400600233547382</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>0.23640000000000003</v>
+        <v>0.1996</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>0.15240078040897356</v>
+        <v>0.16935157802738704</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>0.253</v>
+        <v>0.217</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>0.14264735266233491</v>
+        <v>0.15685915604084727</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>0.26960000000000001</v>
+        <v>0.2344</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>0.13406724448465382</v>
+        <v>0.1460831570001053</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>0.28620000000000001</v>
+        <v>0.25180000000000002</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>0.12646074594019394</v>
+        <v>0.13669257327119996</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>0.30280000000000001</v>
+        <v>0.26919999999999999</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>0.11967103699795384</v>
+        <v>0.12843636840725403</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>0.31940000000000002</v>
+        <v>0.28659999999999997</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>0.11357326036560356</v>
+        <v>0.12112070156829081</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>0.33600000000000002</v>
+        <v>0.30399999999999994</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>0.1080667730805049</v>
+        <v>0.11459351618673833</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>0.35260000000000002</v>
+        <v>0.32139999999999991</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>0.10306954791292257</v>
+        <v>0.10873385691976843</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>0.36920000000000003</v>
+        <v>0.33879999999999988</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>9.8514059456626946E-2</v>
+        <v>0.10344430477692633</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>0.38580000000000003</v>
+        <v>0.35619999999999985</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>9.4344215006141458E-2</v>
+        <v>9.8645517856802326E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>0.40240000000000004</v>
+        <v>0.37359999999999982</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>9.0513033229739207E-2</v>
+        <v>9.4272224250731201E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>0.41900000000000004</v>
+        <v>0.39099999999999979</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>8.6980866365114651E-2</v>
+        <v>9.0270235587773209E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>0.43560000000000004</v>
+        <v>0.40839999999999976</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>8.3714023041660368E-2</v>
+        <v>8.6594190278287006E-2</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>0.45220000000000005</v>
+        <v>0.42579999999999973</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>8.0683690214413156E-2</v>
+        <v>8.3205826588303639E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>0.46880000000000005</v>
+        <v>0.44319999999999971</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>7.786508106536745E-2</v>
+        <v>8.0072645886339167E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>0.48540000000000005</v>
+        <v>0.46059999999999968</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>7.5236755479664214E-2</v>
+        <v>7.7166866949098689E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>0.502</v>
+        <v>0.47799999999999965</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>7.2780073651428162E-2</v>
+        <v>7.4464599978976476E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>0.51859999999999995</v>
+        <v>0.49539999999999962</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>7.0478753352152854E-2</v>
+        <v>7.1945188297737162E-2</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>0.5351999999999999</v>
+        <v>0.51279999999999959</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>6.8318508620103538E-2</v>
+        <v>6.9590679304281408E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>0.55179999999999985</v>
+        <v>0.53019999999999956</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>6.6286752920816941E-2</v>
+        <v>6.7385396022433527E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>0.56839999999999979</v>
+        <v>0.54759999999999953</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>6.4372353744964084E-2</v>
+        <v>6.5315587610704245E-2</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>0.58499999999999974</v>
+        <v>0.5649999999999995</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>6.2565428536686188E-2</v>
+        <v>6.3369142362215705E-2</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>0.60159999999999969</v>
+        <v>0.58239999999999947</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>6.0857174053141214E-2</v>
+        <v>6.1535350536299008E-2</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>0.61819999999999964</v>
+        <v>0.59979999999999944</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>5.9239722935559687E-2</v>
+        <v>5.9804707211371426E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>0.63479999999999959</v>
+        <v>0.61719999999999942</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>5.7706022560319273E-2</v>
+        <v>5.8168747495609484E-2</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>0.65139999999999953</v>
+        <v>0.63459999999999939</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>5.6249732234171644E-2</v>
+        <v>5.6619908064357793E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>0.66799999999999948</v>
+        <v>0.65199999999999936</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>5.4865135572810267E-2</v>
+        <v>5.5151410244589444E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>0.68459999999999943</v>
+        <v>0.66939999999999933</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>5.3547065509446698E-2</v>
+        <v>5.3757160833392201E-2</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>0.70119999999999938</v>
+        <v>0.6867999999999993</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>5.2290839859276121E-2</v>
+        <v>5.2431667589598684E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>0.71779999999999933</v>
+        <v>0.70419999999999927</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>5.1092205746064517E-2</v>
+        <v>5.1169966926928094E-2</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>0.73439999999999928</v>
+        <v>0.72159999999999924</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>4.9947291500731739E-2</v>
+        <v>4.9967561801639478E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>0.75099999999999922</v>
+        <v>0.73899999999999921</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>4.8852564885550918E-2</v>
+        <v>4.8820368156322742E-2</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>0.76759999999999917</v>
+        <v>0.75639999999999918</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>4.7804796694281303E-2</v>
+        <v>4.7724668575619918E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>0.78419999999999912</v>
+        <v>0.77379999999999916</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>4.6801028938076764E-2</v>
+        <v>4.6677072045721392E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>0.80079999999999907</v>
+        <v>0.79119999999999913</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>4.5838546957011887E-2</v>
+        <v>4.5674478899901137E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>0.81739999999999902</v>
+        <v>0.8085999999999991</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>4.4914854903489933E-2</v>
+        <v>4.4714050186738186E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>0.83399999999999896</v>
+        <v>0.82599999999999907</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>4.402765413130065E-2</v>
+        <v>4.379318082343913E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>0.85059999999999891</v>
+        <v>0.84339999999999904</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>4.3174824096344065E-2</v>
+        <v>4.2909475999603458E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>0.86719999999999886</v>
+        <v>0.86079999999999901</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>4.2354405434929264E-2</v>
+        <v>4.2060730381377406E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44">
-        <v>0.88379999999999881</v>
+        <v>0.87819999999999898</v>
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>4.1564584935397719E-2</v>
+        <v>4.1244909735777047E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45">
-        <v>0.90039999999999876</v>
+        <v>0.89559999999999895</v>
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>4.0803682160450119E-2</v>
+        <v>4.0460134652837224E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46">
-        <v>0.91699999999999871</v>
+        <v>0.91299999999999892</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>4.0070137512448881E-2</v>
+        <v>3.9704666091393316E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47">
-        <v>0.93359999999999865</v>
+        <v>0.93039999999999889</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>3.9362501563316381E-2</v>
+        <v>3.8976892514509642E-2</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48">
-        <v>0.9501999999999986</v>
+        <v>0.94779999999999887</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>3.8679425495413117E-2</v>
+        <v>3.8275318414261836E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49">
-        <v>0.96679999999999855</v>
+        <v>0.96519999999999884</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>3.8019652520742214E-2</v>
+        <v>3.7598554053912367E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50">
-        <v>0.9833999999999985</v>
+        <v>0.98259999999999881</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>3.7382010163625065E-2</v>
+        <v>3.6945306279419908E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51">
-        <v>0.99999999999999845</v>
+        <v>0.99999999999999878</v>
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>3.6765403307148836E-2</v>
+        <v>3.6314370272451164E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2352,14 +2341,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3185E053-89BC-4CAE-8FA5-A7C534772840}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>